<commit_message>
line charts - bug fixed
</commit_message>
<xml_diff>
--- a/report_outline.xlsx
+++ b/report_outline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/Data Analytics/6. Country Reports/USA-report-2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2201" documentId="8_{F18DE356-3958-4E61-A81F-20E34B64EA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DB5A4B2-E7F3-4611-8DAD-3BEF2C406525}"/>
+  <xr:revisionPtr revIDLastSave="2209" documentId="8_{F18DE356-3958-4E61-A81F-20E34B64EA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8096DCDC-3367-43AA-9EC9-BA6410ECAEE0}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6B97058B-77ED-4691-9154-36ED9694847A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="348">
   <si>
     <t>Cover</t>
   </si>
@@ -1165,7 +1165,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1193,36 +1193,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1276,7 +1246,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4E37F24-073C-48C0-B5E4-C57E0C193B17}" name="Table1" displayName="Table1" ref="A1:L49" totalsRowShown="0" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4E37F24-073C-48C0-B5E4-C57E0C193B17}" name="Table1" displayName="Table1" ref="A1:L49" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="A1:L49" xr:uid="{F4E37F24-073C-48C0-B5E4-C57E0C193B17}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{D1E86754-498B-4449-AF9C-7F6F91357B29}" name="id"/>
@@ -1287,10 +1257,10 @@
     <tableColumn id="6" xr3:uid="{D78F8B52-A191-41B0-8464-081D07493BD3}" name="section_page"/>
     <tableColumn id="7" xr3:uid="{2C08080F-B5E5-4917-A6E2-1E8583610D91}" name="has_subsection"/>
     <tableColumn id="8" xr3:uid="{268CABA1-2A43-438A-A7EF-385670D18802}" name="thematic_findings"/>
-    <tableColumn id="10" xr3:uid="{B3FC5117-A8E2-4E1B-B517-AAD68F7CB433}" name="title" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{5CC182F6-C715-4AC8-854D-355CB0816969}" name="subtitle" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{224E4B7B-6146-43FA-B490-F87BAA8696E1}" name="footnote" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{4E95668B-FEB8-484F-BB19-1E0983B005D7}" name="macro" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{B3FC5117-A8E2-4E1B-B517-AAD68F7CB433}" name="title" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{5CC182F6-C715-4AC8-854D-355CB0816969}" name="subtitle" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{224E4B7B-6146-43FA-B490-F87BAA8696E1}" name="footnote" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{4E95668B-FEB8-484F-BB19-1E0983B005D7}" name="macro" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1305,7 +1275,7 @@
     <tableColumn id="3" xr3:uid="{B680CB48-28A5-4FB6-98AA-215E22B8B40F}" name="chart_title"/>
     <tableColumn id="4" xr3:uid="{FFEF5F92-2DF3-49A4-BD91-1FA7728CB677}" name="chart_subtitle"/>
     <tableColumn id="5" xr3:uid="{9C01E486-AAA9-4113-9F7C-DFED4772B00B}" name="var_id"/>
-    <tableColumn id="6" xr3:uid="{B447C55F-11C9-4234-9D1F-AF7936BEDF14}" name="reportValues" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{B447C55F-11C9-4234-9D1F-AF7936BEDF14}" name="reportValues" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{3122E94D-312F-487C-A9AD-C0E5E1E51E5E}" name="panel_title"/>
     <tableColumn id="8" xr3:uid="{203C77AD-FB8E-4313-B49E-37F7B9468C14}" name="panel_subtitle"/>
     <tableColumn id="9" xr3:uid="{5273962B-B3E2-440F-8940-B09D8F61305B}" name="type"/>
@@ -1313,7 +1283,7 @@
     <tableColumn id="10" xr3:uid="{DDAEDC79-07D2-402E-81B5-2E1EFAA266FD}" name="legend_text"/>
     <tableColumn id="11" xr3:uid="{2349E397-D3E7-455F-B793-654DDB7A534C}" name="legend_color"/>
     <tableColumn id="12" xr3:uid="{6CA05E5D-08AE-4A36-A0AA-353E1F289F09}" name="sample"/>
-    <tableColumn id="13" xr3:uid="{BCA1C210-6FE1-4DDF-9357-7DAD0B831D61}" name="years" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{BCA1C210-6FE1-4DDF-9357-7DAD0B831D61}" name="years" dataDxfId="3"/>
     <tableColumn id="15" xr3:uid="{79FC7E8F-E231-444D-8CC2-A3A820DFD11C}" name="status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3604,10 +3574,10 @@
   <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N65" sqref="N65"/>
+      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5219,8 +5189,8 @@
       <c r="M34" t="s">
         <v>134</v>
       </c>
-      <c r="N34" s="1">
-        <v>2024</v>
+      <c r="N34" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="O34" t="s">
         <v>347</v>
@@ -5313,8 +5283,8 @@
       <c r="M36" t="s">
         <v>134</v>
       </c>
-      <c r="N36" s="1">
-        <v>2024</v>
+      <c r="N36" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="O36" t="s">
         <v>347</v>
@@ -5971,8 +5941,8 @@
       <c r="M50" t="s">
         <v>134</v>
       </c>
-      <c r="N50" s="1">
-        <v>2024</v>
+      <c r="N50" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="O50" t="s">
         <v>347</v>
@@ -6018,8 +5988,8 @@
       <c r="M51" t="s">
         <v>134</v>
       </c>
-      <c r="N51" s="1">
-        <v>2024</v>
+      <c r="N51" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="O51" t="s">
         <v>347</v>
@@ -6065,8 +6035,8 @@
       <c r="M52" t="s">
         <v>134</v>
       </c>
-      <c r="N52" s="1">
-        <v>2024</v>
+      <c r="N52" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="O52" t="s">
         <v>347</v>
@@ -6112,8 +6082,8 @@
       <c r="M53" t="s">
         <v>134</v>
       </c>
-      <c r="N53" s="1">
-        <v>2024</v>
+      <c r="N53" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="O53" t="s">
         <v>347</v>
@@ -6441,8 +6411,8 @@
       <c r="M60" t="s">
         <v>134</v>
       </c>
-      <c r="N60" s="1">
-        <v>2024</v>
+      <c r="N60" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="O60" t="s">
         <v>347</v>
@@ -6488,8 +6458,8 @@
       <c r="M61" t="s">
         <v>134</v>
       </c>
-      <c r="N61" s="1">
-        <v>2024</v>
+      <c r="N61" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="O61" t="s">
         <v>347</v>
@@ -6535,8 +6505,8 @@
       <c r="M62" t="s">
         <v>134</v>
       </c>
-      <c r="N62" s="1">
-        <v>2024</v>
+      <c r="N62" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="O62" t="s">
         <v>347</v>
@@ -6582,8 +6552,8 @@
       <c r="M63" t="s">
         <v>134</v>
       </c>
-      <c r="N63" s="1">
-        <v>2024</v>
+      <c r="N63" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="O63" t="s">
         <v>347</v>
@@ -7508,14 +7478,14 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O2:O81">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="missing">
-      <formula>NOT(ISERROR(SEARCH("missing",O2)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="coding">
+      <formula>NOT(ISERROR(SEARCH("coding",O2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="ready">
       <formula>NOT(ISERROR(SEARCH("ready",O2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="coding">
-      <formula>NOT(ISERROR(SEARCH("coding",O2)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="missing">
+      <formula>NOT(ISERROR(SEARCH("missing",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7529,26 +7499,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="579d0760968303502ff8eb3a8a5e610f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6855c386bbcb23a4cad2dada315b1779" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
@@ -7797,10 +7747,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBF641CD-F15C-42E5-B454-EB7169F6F499}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99B8D699-284D-4873-A808-FFD96E111D58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7817,20 +7798,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99B8D699-284D-4873-A808-FFD96E111D58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBF641CD-F15C-42E5-B454-EB7169F6F499}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Data Viz up and running
</commit_message>
<xml_diff>
--- a/report_outline.xlsx
+++ b/report_outline.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject-my.sharepoint.com/personal/nclapacs_worldjusticeproject_org/Documents/Documents/GitHub/USA-report-2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/Data Analytics/6. Country Reports/USA-report-2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2372" documentId="8_{F18DE356-3958-4E61-A81F-20E34B64EA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13AADBC0-80DA-44C3-BDFF-AFDE56D873AF}"/>
+  <xr:revisionPtr revIDLastSave="2368" documentId="8_{F18DE356-3958-4E61-A81F-20E34B64EA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5B7AABA-4778-4086-AB74-0670AC003B8F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{6B97058B-77ED-4691-9154-36ED9694847A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="343">
   <si>
     <t>Cover</t>
   </si>
@@ -954,6 +954,21 @@
   </si>
   <si>
     <t>q2g</t>
+  </si>
+  <si>
+    <t>#2a2a95</t>
+  </si>
+  <si>
+    <t>#2a2a96</t>
+  </si>
+  <si>
+    <t>#2a2a97</t>
+  </si>
+  <si>
+    <t>#2a2a98</t>
+  </si>
+  <si>
+    <t>#2a2a99</t>
   </si>
   <si>
     <t>Figure_24</t>
@@ -1166,13 +1181,13 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1190,6 +1205,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/namedSheetViews/namedSheetView1.xml><?xml version="1.0" encoding="utf-8"?>
+<namedSheetViews xmlns="http://schemas.microsoft.com/office/spreadsheetml/2019/namedsheetviews" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14"/>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BA9653AC-F8C3-401C-B349-891D4FF1F533}" name="Table4" displayName="Table4" ref="A1:B6" totalsRowShown="0">
   <autoFilter ref="A1:B6" xr:uid="{BA9653AC-F8C3-401C-B349-891D4FF1F533}"/>
@@ -1202,7 +1225,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4E37F24-073C-48C0-B5E4-C57E0C193B17}" name="Table1" displayName="Table1" ref="A1:J46" totalsRowShown="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4E37F24-073C-48C0-B5E4-C57E0C193B17}" name="Table1" displayName="Table1" ref="A1:J46" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="A1:J46" xr:uid="{F4E37F24-073C-48C0-B5E4-C57E0C193B17}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{D1E86754-498B-4449-AF9C-7F6F91357B29}" name="id"/>
@@ -1214,7 +1237,7 @@
     <tableColumn id="6" xr3:uid="{D78F8B52-A191-41B0-8464-081D07493BD3}" name="section_page"/>
     <tableColumn id="7" xr3:uid="{2C08080F-B5E5-4917-A6E2-1E8583610D91}" name="has_subsection"/>
     <tableColumn id="8" xr3:uid="{268CABA1-2A43-438A-A7EF-385670D18802}" name="thematic_findings"/>
-    <tableColumn id="13" xr3:uid="{4E95668B-FEB8-484F-BB19-1E0983B005D7}" name="macro" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{4E95668B-FEB8-484F-BB19-1E0983B005D7}" name="macro" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1222,20 +1245,14 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{92034C10-9C61-4F8C-87F0-421ACDF97633}" name="Table5" displayName="Table5" ref="A1:P81" totalsRowShown="0">
-  <autoFilter ref="A1:P81" xr:uid="{92034C10-9C61-4F8C-87F0-421ACDF97633}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="Slope"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:P81" xr:uid="{92034C10-9C61-4F8C-87F0-421ACDF97633}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{212EC242-638E-4C2D-8A7C-290B2E57BD74}" name="id"/>
     <tableColumn id="2" xr3:uid="{0605D17D-53ED-4ED7-90F5-CA0A9CEFC8B9}" name="panel"/>
     <tableColumn id="3" xr3:uid="{B680CB48-28A5-4FB6-98AA-215E22B8B40F}" name="chart_title"/>
     <tableColumn id="4" xr3:uid="{FFEF5F92-2DF3-49A4-BD91-1FA7728CB677}" name="chart_subtitle"/>
     <tableColumn id="5" xr3:uid="{9C01E486-AAA9-4113-9F7C-DFED4772B00B}" name="var_id"/>
-    <tableColumn id="6" xr3:uid="{B447C55F-11C9-4234-9D1F-AF7936BEDF14}" name="reportValues" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{B447C55F-11C9-4234-9D1F-AF7936BEDF14}" name="reportValues" dataDxfId="6"/>
     <tableColumn id="7" xr3:uid="{3122E94D-312F-487C-A9AD-C0E5E1E51E5E}" name="panel_title"/>
     <tableColumn id="8" xr3:uid="{203C77AD-FB8E-4313-B49E-37F7B9468C14}" name="panel_subtitle"/>
     <tableColumn id="16" xr3:uid="{121C63F2-C904-48A6-9D20-EC47030AA9FA}" name="footnote"/>
@@ -1244,7 +1261,7 @@
     <tableColumn id="10" xr3:uid="{DDAEDC79-07D2-402E-81B5-2E1EFAA266FD}" name="legend_text"/>
     <tableColumn id="11" xr3:uid="{2349E397-D3E7-455F-B793-654DDB7A534C}" name="legend_color"/>
     <tableColumn id="12" xr3:uid="{6CA05E5D-08AE-4A36-A0AA-353E1F289F09}" name="sample"/>
-    <tableColumn id="13" xr3:uid="{BCA1C210-6FE1-4DDF-9357-7DAD0B831D61}" name="years" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{BCA1C210-6FE1-4DDF-9357-7DAD0B831D61}" name="years" dataDxfId="5"/>
     <tableColumn id="15" xr3:uid="{79FC7E8F-E231-444D-8CC2-A3A820DFD11C}" name="status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1671,7 +1688,7 @@
         <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1947,7 +1964,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1959,7 +1976,7 @@
         <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -2011,7 +2028,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -2023,7 +2040,7 @@
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -2267,7 +2284,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -2279,7 +2296,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -2843,7 +2860,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -2855,7 +2872,7 @@
         <v>26</v>
       </c>
       <c r="E38" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -3143,10 +3160,10 @@
   <dimension ref="A1:P88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomRight" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3199,7 +3216,7 @@
         <v>37</v>
       </c>
       <c r="K1" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="L1" t="s">
         <v>85</v>
@@ -3214,10 +3231,10 @@
         <v>231</v>
       </c>
       <c r="P1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -3264,10 +3281,10 @@
         <v>2024</v>
       </c>
       <c r="P2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -3314,10 +3331,10 @@
         <v>2024</v>
       </c>
       <c r="P3" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>232</v>
       </c>
@@ -3349,7 +3366,7 @@
         <v>258</v>
       </c>
       <c r="K4" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L4" t="s">
         <v>190</v>
@@ -3364,10 +3381,10 @@
         <v>2024</v>
       </c>
       <c r="P4" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -3399,7 +3416,7 @@
         <v>258</v>
       </c>
       <c r="K5" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L5" t="s">
         <v>190</v>
@@ -3414,10 +3431,10 @@
         <v>2024</v>
       </c>
       <c r="P5" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>232</v>
       </c>
@@ -3449,7 +3466,7 @@
         <v>258</v>
       </c>
       <c r="K6" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L6" t="s">
         <v>190</v>
@@ -3464,10 +3481,10 @@
         <v>2024</v>
       </c>
       <c r="P6" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -3499,7 +3516,7 @@
         <v>263</v>
       </c>
       <c r="K7" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L7" t="s">
         <v>12</v>
@@ -3514,10 +3531,10 @@
         <v>237</v>
       </c>
       <c r="P7" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -3555,7 +3572,7 @@
         <v>289</v>
       </c>
       <c r="M8" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="N8" t="s">
         <v>190</v>
@@ -3564,10 +3581,10 @@
         <v>289</v>
       </c>
       <c r="P8" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>235</v>
       </c>
@@ -3614,10 +3631,10 @@
         <v>2024</v>
       </c>
       <c r="P9" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -3631,7 +3648,7 @@
         <v>278</v>
       </c>
       <c r="E10" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>239</v>
@@ -3646,10 +3663,10 @@
         <v>12</v>
       </c>
       <c r="J10" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="K10" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L10" t="s">
         <v>12</v>
@@ -3664,10 +3681,10 @@
         <v>2024</v>
       </c>
       <c r="P10" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -3681,13 +3698,13 @@
         <v>278</v>
       </c>
       <c r="E11" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>239</v>
       </c>
       <c r="G11" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="H11" t="s">
         <v>12</v>
@@ -3696,10 +3713,10 @@
         <v>12</v>
       </c>
       <c r="J11" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="K11" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L11" t="s">
         <v>12</v>
@@ -3714,10 +3731,10 @@
         <v>2024</v>
       </c>
       <c r="P11" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -3731,13 +3748,13 @@
         <v>278</v>
       </c>
       <c r="E12" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>239</v>
       </c>
       <c r="G12" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="H12" t="s">
         <v>12</v>
@@ -3746,10 +3763,10 @@
         <v>12</v>
       </c>
       <c r="J12" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="K12" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L12" t="s">
         <v>12</v>
@@ -3764,10 +3781,10 @@
         <v>2024</v>
       </c>
       <c r="P12" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -3781,13 +3798,13 @@
         <v>278</v>
       </c>
       <c r="E13" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>239</v>
       </c>
       <c r="G13" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="H13" t="s">
         <v>12</v>
@@ -3796,10 +3813,10 @@
         <v>12</v>
       </c>
       <c r="J13" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="K13" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L13" t="s">
         <v>12</v>
@@ -3814,10 +3831,10 @@
         <v>2024</v>
       </c>
       <c r="P13" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -3831,7 +3848,7 @@
         <v>278</v>
       </c>
       <c r="E14" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>239</v>
@@ -3849,7 +3866,7 @@
         <v>260</v>
       </c>
       <c r="K14" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L14" t="s">
         <v>190</v>
@@ -3864,10 +3881,10 @@
         <v>2024</v>
       </c>
       <c r="P14" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -3881,13 +3898,13 @@
         <v>278</v>
       </c>
       <c r="E15" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>239</v>
       </c>
       <c r="G15" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="H15" t="s">
         <v>12</v>
@@ -3899,7 +3916,7 @@
         <v>260</v>
       </c>
       <c r="K15" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L15" t="s">
         <v>190</v>
@@ -3914,10 +3931,10 @@
         <v>2024</v>
       </c>
       <c r="P15" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -3931,13 +3948,13 @@
         <v>278</v>
       </c>
       <c r="E16" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>239</v>
       </c>
       <c r="G16" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="H16" t="s">
         <v>12</v>
@@ -3949,7 +3966,7 @@
         <v>260</v>
       </c>
       <c r="K16" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L16" t="s">
         <v>190</v>
@@ -3964,10 +3981,10 @@
         <v>2024</v>
       </c>
       <c r="P16" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -3981,13 +3998,13 @@
         <v>278</v>
       </c>
       <c r="E17" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>239</v>
       </c>
       <c r="G17" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="H17" t="s">
         <v>12</v>
@@ -3999,7 +4016,7 @@
         <v>260</v>
       </c>
       <c r="K17" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L17" t="s">
         <v>190</v>
@@ -4014,10 +4031,10 @@
         <v>2024</v>
       </c>
       <c r="P17" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -4064,10 +4081,10 @@
         <v>2024</v>
       </c>
       <c r="P18" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -4099,7 +4116,7 @@
         <v>264</v>
       </c>
       <c r="K19" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L19" t="s">
         <v>190</v>
@@ -4114,10 +4131,10 @@
         <v>2024</v>
       </c>
       <c r="P19" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -4128,7 +4145,7 @@
         <v>120</v>
       </c>
       <c r="D20" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="E20" t="s">
         <v>241</v>
@@ -4149,7 +4166,7 @@
         <v>264</v>
       </c>
       <c r="K20" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L20" t="s">
         <v>190</v>
@@ -4164,10 +4181,10 @@
         <v>2024</v>
       </c>
       <c r="P20" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>250</v>
       </c>
@@ -4199,7 +4216,7 @@
         <v>263</v>
       </c>
       <c r="K21" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L21" t="s">
         <v>12</v>
@@ -4214,10 +4231,10 @@
         <v>237</v>
       </c>
       <c r="P21" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>251</v>
       </c>
@@ -4264,10 +4281,10 @@
         <v>2024</v>
       </c>
       <c r="P22" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>240</v>
       </c>
@@ -4299,7 +4316,7 @@
         <v>258</v>
       </c>
       <c r="K23" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L23" t="s">
         <v>190</v>
@@ -4314,10 +4331,10 @@
         <v>2024</v>
       </c>
       <c r="P23" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>240</v>
       </c>
@@ -4349,7 +4366,7 @@
         <v>258</v>
       </c>
       <c r="K24" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L24" t="s">
         <v>190</v>
@@ -4364,10 +4381,10 @@
         <v>2024</v>
       </c>
       <c r="P24" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>240</v>
       </c>
@@ -4399,7 +4416,7 @@
         <v>258</v>
       </c>
       <c r="K25" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L25" t="s">
         <v>190</v>
@@ -4414,10 +4431,10 @@
         <v>2024</v>
       </c>
       <c r="P25" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -4449,10 +4466,10 @@
         <v>262</v>
       </c>
       <c r="K26" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L26" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="M26" t="s">
         <v>172</v>
@@ -4464,10 +4481,10 @@
         <v>2024</v>
       </c>
       <c r="P26" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -4499,10 +4516,10 @@
         <v>262</v>
       </c>
       <c r="K27" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L27" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="M27" t="s">
         <v>172</v>
@@ -4514,10 +4531,10 @@
         <v>2024</v>
       </c>
       <c r="P27" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -4549,10 +4566,10 @@
         <v>262</v>
       </c>
       <c r="K28" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L28" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="M28" t="s">
         <v>172</v>
@@ -4564,10 +4581,10 @@
         <v>2024</v>
       </c>
       <c r="P28" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -4599,10 +4616,10 @@
         <v>262</v>
       </c>
       <c r="K29" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="M29" t="s">
         <v>172</v>
@@ -4614,10 +4631,10 @@
         <v>2024</v>
       </c>
       <c r="P29" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -4649,10 +4666,10 @@
         <v>262</v>
       </c>
       <c r="K30" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L30" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="M30" t="s">
         <v>172</v>
@@ -4664,7 +4681,7 @@
         <v>2024</v>
       </c>
       <c r="P30" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
@@ -4699,13 +4716,13 @@
         <v>243</v>
       </c>
       <c r="K31" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L31" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M31" t="s">
-        <v>102</v>
+        <v>172</v>
       </c>
       <c r="N31" t="s">
         <v>190</v>
@@ -4714,7 +4731,7 @@
         <v>289</v>
       </c>
       <c r="P31" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
@@ -4749,13 +4766,13 @@
         <v>243</v>
       </c>
       <c r="K32" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L32" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M32" t="s">
-        <v>102</v>
+        <v>172</v>
       </c>
       <c r="N32" t="s">
         <v>190</v>
@@ -4764,7 +4781,7 @@
         <v>289</v>
       </c>
       <c r="P32" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.35">
@@ -4799,13 +4816,13 @@
         <v>243</v>
       </c>
       <c r="K33" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L33" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M33" t="s">
-        <v>102</v>
+        <v>172</v>
       </c>
       <c r="N33" t="s">
         <v>190</v>
@@ -4814,10 +4831,10 @@
         <v>289</v>
       </c>
       <c r="P33" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -4849,7 +4866,7 @@
         <v>263</v>
       </c>
       <c r="K34" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L34" t="s">
         <v>12</v>
@@ -4864,7 +4881,7 @@
         <v>237</v>
       </c>
       <c r="P34" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
@@ -4899,7 +4916,7 @@
         <v>243</v>
       </c>
       <c r="K35" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L35" t="s">
         <v>190</v>
@@ -4914,10 +4931,10 @@
         <v>289</v>
       </c>
       <c r="P35" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -4949,7 +4966,7 @@
         <v>263</v>
       </c>
       <c r="K36" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L36" t="s">
         <v>12</v>
@@ -4964,7 +4981,7 @@
         <v>237</v>
       </c>
       <c r="P36" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
@@ -4999,7 +5016,7 @@
         <v>243</v>
       </c>
       <c r="K37" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L37" t="s">
         <v>190</v>
@@ -5014,10 +5031,10 @@
         <v>289</v>
       </c>
       <c r="P37" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>293</v>
       </c>
@@ -5049,7 +5066,7 @@
         <v>263</v>
       </c>
       <c r="K38" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L38" t="s">
         <v>12</v>
@@ -5064,10 +5081,10 @@
         <v>237</v>
       </c>
       <c r="P38" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>293</v>
       </c>
@@ -5099,7 +5116,7 @@
         <v>263</v>
       </c>
       <c r="K39" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L39" t="s">
         <v>12</v>
@@ -5114,10 +5131,10 @@
         <v>237</v>
       </c>
       <c r="P39" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>293</v>
       </c>
@@ -5149,7 +5166,7 @@
         <v>263</v>
       </c>
       <c r="K40" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L40" t="s">
         <v>12</v>
@@ -5164,10 +5181,10 @@
         <v>237</v>
       </c>
       <c r="P40" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>293</v>
       </c>
@@ -5199,7 +5216,7 @@
         <v>263</v>
       </c>
       <c r="K41" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L41" t="s">
         <v>12</v>
@@ -5214,10 +5231,10 @@
         <v>237</v>
       </c>
       <c r="P41" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>293</v>
       </c>
@@ -5249,7 +5266,7 @@
         <v>263</v>
       </c>
       <c r="K42" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L42" t="s">
         <v>12</v>
@@ -5264,10 +5281,10 @@
         <v>237</v>
       </c>
       <c r="P42" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>294</v>
       </c>
@@ -5299,7 +5316,7 @@
         <v>263</v>
       </c>
       <c r="K43" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L43" t="s">
         <v>12</v>
@@ -5314,10 +5331,10 @@
         <v>237</v>
       </c>
       <c r="P43" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>294</v>
       </c>
@@ -5349,7 +5366,7 @@
         <v>263</v>
       </c>
       <c r="K44" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L44" t="s">
         <v>12</v>
@@ -5364,10 +5381,10 @@
         <v>237</v>
       </c>
       <c r="P44" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>294</v>
       </c>
@@ -5399,7 +5416,7 @@
         <v>263</v>
       </c>
       <c r="K45" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L45" t="s">
         <v>12</v>
@@ -5414,10 +5431,10 @@
         <v>237</v>
       </c>
       <c r="P45" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>294</v>
       </c>
@@ -5449,7 +5466,7 @@
         <v>263</v>
       </c>
       <c r="K46" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L46" t="s">
         <v>12</v>
@@ -5464,10 +5481,10 @@
         <v>237</v>
       </c>
       <c r="P46" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>294</v>
       </c>
@@ -5499,7 +5516,7 @@
         <v>263</v>
       </c>
       <c r="K47" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L47" t="s">
         <v>12</v>
@@ -5514,10 +5531,10 @@
         <v>237</v>
       </c>
       <c r="P47" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>294</v>
       </c>
@@ -5549,7 +5566,7 @@
         <v>263</v>
       </c>
       <c r="K48" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L48" t="s">
         <v>12</v>
@@ -5564,10 +5581,10 @@
         <v>237</v>
       </c>
       <c r="P48" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -5599,7 +5616,7 @@
         <v>264</v>
       </c>
       <c r="K49" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L49" t="s">
         <v>190</v>
@@ -5614,10 +5631,10 @@
         <v>2024</v>
       </c>
       <c r="P49" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -5649,7 +5666,7 @@
         <v>263</v>
       </c>
       <c r="K50" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L50" t="s">
         <v>12</v>
@@ -5664,10 +5681,10 @@
         <v>237</v>
       </c>
       <c r="P50" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -5699,7 +5716,7 @@
         <v>263</v>
       </c>
       <c r="K51" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L51" t="s">
         <v>12</v>
@@ -5714,10 +5731,10 @@
         <v>237</v>
       </c>
       <c r="P51" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -5749,7 +5766,7 @@
         <v>263</v>
       </c>
       <c r="K52" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L52" t="s">
         <v>191</v>
@@ -5764,10 +5781,10 @@
         <v>237</v>
       </c>
       <c r="P52" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -5799,7 +5816,7 @@
         <v>263</v>
       </c>
       <c r="K53" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L53" t="s">
         <v>192</v>
@@ -5814,7 +5831,7 @@
         <v>237</v>
       </c>
       <c r="P53" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
@@ -5849,13 +5866,13 @@
         <v>243</v>
       </c>
       <c r="K54" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L54" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M54" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="N54" t="s">
         <v>190</v>
@@ -5864,7 +5881,7 @@
         <v>289</v>
       </c>
       <c r="P54" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
@@ -5899,13 +5916,13 @@
         <v>243</v>
       </c>
       <c r="K55" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L55" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M55" t="s">
-        <v>102</v>
+        <v>304</v>
       </c>
       <c r="N55" t="s">
         <v>190</v>
@@ -5914,7 +5931,7 @@
         <v>289</v>
       </c>
       <c r="P55" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.35">
@@ -5949,13 +5966,13 @@
         <v>243</v>
       </c>
       <c r="K56" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L56" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M56" t="s">
-        <v>102</v>
+        <v>305</v>
       </c>
       <c r="N56" t="s">
         <v>190</v>
@@ -5964,7 +5981,7 @@
         <v>289</v>
       </c>
       <c r="P56" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
@@ -5999,13 +6016,13 @@
         <v>243</v>
       </c>
       <c r="K57" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L57" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M57" t="s">
-        <v>102</v>
+        <v>306</v>
       </c>
       <c r="N57" t="s">
         <v>190</v>
@@ -6014,7 +6031,7 @@
         <v>289</v>
       </c>
       <c r="P57" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
@@ -6049,13 +6066,13 @@
         <v>243</v>
       </c>
       <c r="K58" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L58" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M58" t="s">
-        <v>102</v>
+        <v>307</v>
       </c>
       <c r="N58" t="s">
         <v>190</v>
@@ -6064,7 +6081,7 @@
         <v>289</v>
       </c>
       <c r="P58" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
@@ -6099,13 +6116,13 @@
         <v>243</v>
       </c>
       <c r="K59" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L59" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M59" t="s">
-        <v>102</v>
+        <v>308</v>
       </c>
       <c r="N59" t="s">
         <v>190</v>
@@ -6114,10 +6131,10 @@
         <v>289</v>
       </c>
       <c r="P59" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -6149,7 +6166,7 @@
         <v>263</v>
       </c>
       <c r="K60" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L60" t="s">
         <v>12</v>
@@ -6164,10 +6181,10 @@
         <v>237</v>
       </c>
       <c r="P60" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -6199,7 +6216,7 @@
         <v>263</v>
       </c>
       <c r="K61" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L61" t="s">
         <v>12</v>
@@ -6214,10 +6231,10 @@
         <v>237</v>
       </c>
       <c r="P61" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -6249,7 +6266,7 @@
         <v>263</v>
       </c>
       <c r="K62" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L62" t="s">
         <v>191</v>
@@ -6264,10 +6281,10 @@
         <v>237</v>
       </c>
       <c r="P62" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -6299,7 +6316,7 @@
         <v>263</v>
       </c>
       <c r="K63" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L63" t="s">
         <v>192</v>
@@ -6314,7 +6331,7 @@
         <v>237</v>
       </c>
       <c r="P63" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
@@ -6325,7 +6342,7 @@
         <v>87</v>
       </c>
       <c r="C64" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="D64" t="s">
         <v>168</v>
@@ -6349,13 +6366,13 @@
         <v>243</v>
       </c>
       <c r="K64" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L64" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M64" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="N64" t="s">
         <v>190</v>
@@ -6364,7 +6381,7 @@
         <v>289</v>
       </c>
       <c r="P64" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.35">
@@ -6375,19 +6392,19 @@
         <v>88</v>
       </c>
       <c r="C65" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="D65" t="s">
         <v>168</v>
       </c>
       <c r="E65" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>239</v>
       </c>
       <c r="G65" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="H65" t="s">
         <v>12</v>
@@ -6399,13 +6416,13 @@
         <v>243</v>
       </c>
       <c r="K65" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L65" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M65" t="s">
-        <v>102</v>
+        <v>304</v>
       </c>
       <c r="N65" t="s">
         <v>190</v>
@@ -6414,7 +6431,7 @@
         <v>289</v>
       </c>
       <c r="P65" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.35">
@@ -6425,13 +6442,13 @@
         <v>94</v>
       </c>
       <c r="C66" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="D66" t="s">
         <v>168</v>
       </c>
       <c r="E66" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>239</v>
@@ -6449,13 +6466,13 @@
         <v>243</v>
       </c>
       <c r="K66" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L66" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M66" t="s">
-        <v>102</v>
+        <v>305</v>
       </c>
       <c r="N66" t="s">
         <v>190</v>
@@ -6464,7 +6481,7 @@
         <v>289</v>
       </c>
       <c r="P66" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.35">
@@ -6475,13 +6492,13 @@
         <v>114</v>
       </c>
       <c r="C67" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="D67" t="s">
         <v>168</v>
       </c>
       <c r="E67" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>239</v>
@@ -6499,13 +6516,13 @@
         <v>243</v>
       </c>
       <c r="K67" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L67" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M67" t="s">
-        <v>102</v>
+        <v>306</v>
       </c>
       <c r="N67" t="s">
         <v>190</v>
@@ -6514,7 +6531,7 @@
         <v>289</v>
       </c>
       <c r="P67" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.35">
@@ -6525,13 +6542,13 @@
         <v>126</v>
       </c>
       <c r="C68" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="D68" t="s">
         <v>168</v>
       </c>
       <c r="E68" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>239</v>
@@ -6549,13 +6566,13 @@
         <v>243</v>
       </c>
       <c r="K68" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L68" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M68" t="s">
-        <v>102</v>
+        <v>307</v>
       </c>
       <c r="N68" t="s">
         <v>190</v>
@@ -6564,7 +6581,7 @@
         <v>289</v>
       </c>
       <c r="P68" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.35">
@@ -6575,13 +6592,13 @@
         <v>135</v>
       </c>
       <c r="C69" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="D69" t="s">
         <v>168</v>
       </c>
       <c r="E69" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>239</v>
@@ -6599,13 +6616,13 @@
         <v>243</v>
       </c>
       <c r="K69" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L69" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="M69" t="s">
-        <v>102</v>
+        <v>308</v>
       </c>
       <c r="N69" t="s">
         <v>190</v>
@@ -6614,10 +6631,10 @@
         <v>289</v>
       </c>
       <c r="P69" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>62</v>
       </c>
@@ -6649,13 +6666,13 @@
         <v>261</v>
       </c>
       <c r="K70" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L70" s="7" t="s">
         <v>289</v>
       </c>
       <c r="M70" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="N70" t="s">
         <v>131</v>
@@ -6664,10 +6681,10 @@
         <v>289</v>
       </c>
       <c r="P70" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>62</v>
       </c>
@@ -6699,13 +6716,13 @@
         <v>261</v>
       </c>
       <c r="K71" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L71" s="7" t="s">
         <v>289</v>
       </c>
       <c r="M71" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="N71" t="s">
         <v>131</v>
@@ -6714,10 +6731,10 @@
         <v>289</v>
       </c>
       <c r="P71" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>62</v>
       </c>
@@ -6749,13 +6766,13 @@
         <v>261</v>
       </c>
       <c r="K72" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L72" s="7" t="s">
         <v>289</v>
       </c>
       <c r="M72" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="N72" t="s">
         <v>131</v>
@@ -6764,10 +6781,10 @@
         <v>289</v>
       </c>
       <c r="P72" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>63</v>
       </c>
@@ -6799,7 +6816,7 @@
         <v>260</v>
       </c>
       <c r="K73" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L73" s="7" t="s">
         <v>190</v>
@@ -6814,10 +6831,10 @@
         <v>2024</v>
       </c>
       <c r="P73" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -6849,7 +6866,7 @@
         <v>260</v>
       </c>
       <c r="K74" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L74" t="s">
         <v>190</v>
@@ -6864,10 +6881,10 @@
         <v>2024</v>
       </c>
       <c r="P74" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>63</v>
       </c>
@@ -6899,7 +6916,7 @@
         <v>260</v>
       </c>
       <c r="K75" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="L75" t="s">
         <v>190</v>
@@ -6914,10 +6931,10 @@
         <v>2024</v>
       </c>
       <c r="P75" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>64</v>
       </c>
@@ -6949,7 +6966,7 @@
         <v>263</v>
       </c>
       <c r="K76" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L76" t="s">
         <v>193</v>
@@ -6964,10 +6981,10 @@
         <v>237</v>
       </c>
       <c r="P76" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>64</v>
       </c>
@@ -6999,7 +7016,7 @@
         <v>263</v>
       </c>
       <c r="K77" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L77" t="s">
         <v>193</v>
@@ -7014,10 +7031,10 @@
         <v>237</v>
       </c>
       <c r="P77" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>64</v>
       </c>
@@ -7049,7 +7066,7 @@
         <v>263</v>
       </c>
       <c r="K78" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L78" t="s">
         <v>193</v>
@@ -7064,12 +7081,12 @@
         <v>237</v>
       </c>
       <c r="P78" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="B79" t="s">
         <v>87</v>
@@ -7099,7 +7116,7 @@
         <v>243</v>
       </c>
       <c r="K79" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L79" t="s">
         <v>190</v>
@@ -7114,12 +7131,12 @@
         <v>289</v>
       </c>
       <c r="P79" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="B80" t="s">
         <v>88</v>
@@ -7149,7 +7166,7 @@
         <v>243</v>
       </c>
       <c r="K80" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L80" t="s">
         <v>190</v>
@@ -7164,12 +7181,12 @@
         <v>289</v>
       </c>
       <c r="P80" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="B81" t="s">
         <v>94</v>
@@ -7199,7 +7216,7 @@
         <v>243</v>
       </c>
       <c r="K81" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="L81" t="s">
         <v>190</v>
@@ -7214,7 +7231,7 @@
         <v>289</v>
       </c>
       <c r="P81" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.35">
@@ -7318,17 +7335,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="579d0760968303502ff8eb3a8a5e610f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6855c386bbcb23a4cad2dada315b1779" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
@@ -7577,6 +7583,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7587,17 +7604,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1EE7D2B-72B9-4B29-A99A-A2518AB2EE2A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99B8D699-284D-4873-A808-FFD96E111D58}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7616,6 +7622,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1EE7D2B-72B9-4B29-A99A-A2518AB2EE2A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBF641CD-F15C-42E5-B454-EB7169F6F499}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
adding appendix and methodology
</commit_message>
<xml_diff>
--- a/report_outline.xlsx
+++ b/report_outline.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/Data Analytics/6. Country Reports/USA-report-2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject-my.sharepoint.com/personal/icoddington_worldjusticeproject_org/Documents/Desktop/Github/USA-report-2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2863" documentId="8_{F18DE356-3958-4E61-A81F-20E34B64EA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CF65E18-4C64-4DFD-9601-4B4D75055CC9}"/>
+  <xr:revisionPtr revIDLastSave="2972" documentId="8_{F18DE356-3958-4E61-A81F-20E34B64EA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A034C900-80C7-4C33-9E0D-CCFF80C295D8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6B97058B-77ED-4691-9154-36ED9694847A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{6B97058B-77ED-4691-9154-36ED9694847A}"/>
   </bookViews>
   <sheets>
     <sheet name="general_info" sheetId="3" r:id="rId1"/>
     <sheet name="outline" sheetId="5" r:id="rId2"/>
-    <sheet name="figure_map" sheetId="4" r:id="rId3"/>
+    <sheet name="other_publications" sheetId="6" r:id="rId3"/>
+    <sheet name="methodological_materials" sheetId="7" r:id="rId4"/>
+    <sheet name="figure_map" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="261">
   <si>
     <t>Cover</t>
   </si>
@@ -725,13 +727,121 @@
   </si>
   <si>
     <t xml:space="preserve">Percentage of respondents that would or would not accept the election results in the following scenarios... </t>
+  </si>
+  <si>
+    <t>onClick</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>href</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>WJP Rule of Law Index 2022 Insights</t>
+  </si>
+  <si>
+    <t>https://worldjusticeproject.mx/wp-content/uploads/2022/05/1_WJP_IEDMX_Digital.pdf</t>
+  </si>
+  <si>
+    <r>
+      <t>https</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>://worldjusticeproject.mx/wp-content/uploads/2022/05/1_WJP_IEDMX_Digital.pdf</t>
+    </r>
+  </si>
+  <si>
+    <t>material_name</t>
+  </si>
+  <si>
+    <t>GENERAL POPULATION POLL (GPP)</t>
+  </si>
+  <si>
+    <t>https://worldjusticeproject.org/sites/default/files/documents/South%20America%20GPP%20Questionnaire%202022_English.pdf</t>
+  </si>
+  <si>
+    <t>World Justice Project General Population Poll 2022 – South American Survey Instrument (English Versions A &amp; B)</t>
+  </si>
+  <si>
+    <t>The General Population Poll in South America was designed to capture high-quality data on the realities and concerns of ordinary people on a variety of themes related to the rule of law, including authoritarianism, government accountability, bribery, corruption, police performance, crime and security, and access to justice.  </t>
+  </si>
+  <si>
+    <t>VARIABLES USED IN INFOGRAPHICS ON CRIME VICTIMIZATION</t>
+  </si>
+  <si>
+    <t>This table lists the question-level variables from the General Population Poll used to construct Chart 12.1 and the “Reasons the crime was not reported” table in Chart 12.2.</t>
+  </si>
+  <si>
+    <t>https://worldjusticeproject.org/sites/default/files/documents/Crime%20Victimization%20Variable%20Map_South%20America.pdf</t>
+  </si>
+  <si>
+    <t>World Justice Project Crime Rates and Reporting Variable Map</t>
+  </si>
+  <si>
+    <t>REGRESSION TABLES FOR REGRESSION ANALYSIS USED IN INFOGRAPHIC ON PERCEPTIONS OF SECURITY</t>
+  </si>
+  <si>
+    <t>This document includes the question-level variables from the General Population Poll used in the regression analysis and the regression results featured in Chart 13.2.</t>
+  </si>
+  <si>
+    <t>https://worldjusticeproject.org/sites/default/files/documents/Regression%20Tables_South%20America_0.pdf</t>
+  </si>
+  <si>
+    <t>World Justice Project Regression Tables</t>
+  </si>
+  <si>
+    <t>link1</t>
+  </si>
+  <si>
+    <t>label1</t>
+  </si>
+  <si>
+    <t>link2</t>
+  </si>
+  <si>
+    <t>label2</t>
+  </si>
+  <si>
+    <t>Rule of Law in North Macedonia -- 2023</t>
+  </si>
+  <si>
+    <t>static/charts_and_images/imgPublications/rule_law_index_2022_insights.png</t>
+  </si>
+  <si>
+    <t>https://worldjusticeproject.org/our-work/research-and-data/rule-of-law/north-macedonia-2023</t>
+  </si>
+  <si>
+    <t>static/charts_and_images/imgPublications/bg-cover.jpg</t>
+  </si>
+  <si>
+    <t>static/charts_and_images/imgPublications/ROLI-Insights.png</t>
+  </si>
+  <si>
+    <t>https://worldjusticeproject.org/rule-of-law-index/global/2023</t>
+  </si>
+  <si>
+    <t>WJP Rule of Law Index 2023 Insights</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -741,6 +851,35 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -769,10 +908,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -784,11 +924,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -826,6 +978,270 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -844,6 +1260,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BA9653AC-F8C3-401C-B349-891D4FF1F533}" name="Table4" displayName="Table4" ref="A1:B6" totalsRowShown="0">
   <autoFilter ref="A1:B6" xr:uid="{BA9653AC-F8C3-401C-B349-891D4FF1F533}"/>
@@ -856,7 +1276,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8B14E03D-B076-4E47-842E-3221DD393923}" name="Table14" displayName="Table14" ref="A1:K29" totalsRowShown="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8B14E03D-B076-4E47-842E-3221DD393923}" name="Table14" displayName="Table14" ref="A1:K29" totalsRowShown="0" dataDxfId="20">
   <autoFilter ref="A1:K29" xr:uid="{8B14E03D-B076-4E47-842E-3221DD393923}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{9CFB6294-2D1F-459C-958F-167AA1ADC69D}" name="id"/>
@@ -869,13 +1289,41 @@
     <tableColumn id="7" xr3:uid="{7D4CCB54-6DC7-4469-A234-60DD891FC399}" name="has_subsection"/>
     <tableColumn id="8" xr3:uid="{69BC0A78-B535-4CFE-92C3-285DED5D7490}" name="thematic_findings"/>
     <tableColumn id="9" xr3:uid="{D81CCAC3-A209-46F3-88C1-0250B379E958}" name="legend"/>
-    <tableColumn id="13" xr3:uid="{D4941AAA-948A-4C26-9998-E656071F295A}" name="macro" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{D4941AAA-948A-4C26-9998-E656071F295A}" name="macro" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ACB93786-F805-4D77-91EF-7E8E15DFC5F9}" name="Table1" displayName="Table1" ref="A1:D4" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:D4" xr:uid="{ACB93786-F805-4D77-91EF-7E8E15DFC5F9}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0E8B927F-EDA3-44B5-A65F-A43249F8CEFA}" name="onClick" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{37F3D23E-B415-4A3B-8597-71D6413E2E7C}" name="img" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{148497E4-B1E5-47F7-AE41-6BCCE6689F43}" name="href" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{3CC541A0-1A30-4765-BCDB-703BB62E0CFF}" name="text" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1493FFEA-D985-4ADD-8712-2894823646AD}" name="Table5" displayName="Table5" ref="A1:F4" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:F4" xr:uid="{1493FFEA-D985-4ADD-8712-2894823646AD}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{93B89B02-E871-4E2D-8436-6488CD60EF55}" name="material_name" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{07B3A73C-6FB0-47EA-9648-DBDE4BDCF460}" name="description" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{4F00246D-2D81-438C-B4FA-295885A0001B}" name="link1" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{90681B1B-22F0-456F-8696-E186F2FC350B}" name="label1" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{1AE75421-366F-4379-8983-5CF8141CE424}" name="link2" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{95F573B3-309B-4A0A-A474-6A955D9D59DA}" name="label2" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4E522B1-3123-499E-83E5-BBB41A9C0B72}" name="Table53" displayName="Table53" ref="A1:Q42" totalsRowShown="0">
   <autoFilter ref="A1:Q42" xr:uid="{F4E522B1-3123-499E-83E5-BBB41A9C0B72}"/>
   <tableColumns count="17">
@@ -1224,13 +1672,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="2" width="99.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="99.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1238,7 +1686,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1246,7 +1694,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1254,7 +1702,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -1262,7 +1710,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1270,7 +1718,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1290,20 +1738,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B32341-F9AC-424D-8D69-9ABCF2FF7D4F}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="50.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.08984375" customWidth="1"/>
+    <col min="3" max="3" width="50.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1338,7 +1786,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1408,7 +1856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1443,7 +1891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1478,7 +1926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1513,7 +1961,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -1548,7 +1996,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -1583,7 +2031,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1618,7 +2066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1653,7 +2101,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>184</v>
       </c>
@@ -1688,7 +2136,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -1723,7 +2171,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1758,7 +2206,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1793,7 +2241,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1828,7 +2276,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1863,7 +2311,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1898,7 +2346,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1933,7 +2381,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>183</v>
       </c>
@@ -1968,7 +2416,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>129</v>
       </c>
@@ -2003,7 +2451,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2038,7 +2486,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -2073,7 +2521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2108,7 +2556,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2143,7 +2591,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2178,7 +2626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -2213,7 +2661,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -2248,7 +2696,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2283,7 +2731,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2328,25 +2776,216 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B777675-D9D1-464A-8253-1276A291F711}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.7265625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{DDE09507-FDBB-4B92-A1BB-6B5D8A472EAA}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{9AF91C49-C50E-4740-B8B2-B2601753393F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3769AE-46C0-4DAC-98E3-FE5BCEAF61EE}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.90625" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8942074E-1171-4680-A697-1A8E37014FFA}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="M27" sqref="M21:M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2399,7 +3038,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>185</v>
       </c>
@@ -2452,7 +3091,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>122</v>
       </c>
@@ -2505,7 +3144,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>122</v>
       </c>
@@ -2558,7 +3197,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>122</v>
       </c>
@@ -2611,7 +3250,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -2664,7 +3303,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -2717,7 +3356,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -2770,7 +3409,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -2823,7 +3462,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -2876,7 +3515,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -2929,7 +3568,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -2982,7 +3621,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -3035,7 +3674,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -3088,7 +3727,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -3141,7 +3780,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -3191,7 +3830,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -3244,7 +3883,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -3297,7 +3936,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -3350,7 +3989,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -3403,7 +4042,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -3456,7 +4095,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -3509,7 +4148,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -3562,7 +4201,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -3615,7 +4254,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -3668,7 +4307,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -3721,7 +4360,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -3774,7 +4413,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -3827,7 +4466,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -3880,7 +4519,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -3933,7 +4572,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>183</v>
       </c>
@@ -3986,7 +4625,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>129</v>
       </c>
@@ -4039,7 +4678,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
@@ -4092,7 +4731,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
@@ -4145,7 +4784,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>43</v>
       </c>
@@ -4198,7 +4837,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>43</v>
       </c>
@@ -4251,7 +4890,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>43</v>
       </c>
@@ -4304,7 +4943,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -4357,7 +4996,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -4410,7 +5049,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
@@ -4463,7 +5102,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>43</v>
       </c>
@@ -4516,7 +5155,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>

</xml_diff>